<commit_message>
modal summary correction vol3
</commit_message>
<xml_diff>
--- a/data/excel/802576637_2025_invoices.xlsx
+++ b/data/excel/802576637_2025_invoices.xlsx
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>400011186892779</t>
+          <t>400011172559639</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -508,17 +508,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>8Μ0ΤΔΑ</t>
+          <t>12Μ0ΤΔΑ</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>8970</t>
+          <t>10768</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>04/10/2025</t>
+          <t>03/10/2025</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -529,17 +529,17 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>48,39</t>
+          <t>13,83</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>11,61</t>
+          <t>3,32</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>60,00</t>
+          <t>17,15</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modal summary correction vol4
</commit_message>
<xml_diff>
--- a/data/excel/802576637_2025_invoices.xlsx
+++ b/data/excel/802576637_2025_invoices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,51 @@
           <t>Σύνολο</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>issueDate</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>AFM_issuer</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>series</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>totalNetValue</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>totalVatAmount</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>totalValue</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>character</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -542,6 +587,77 @@
           <t>17,15</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>400011184530011</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>094439854</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>5Μ0ΤΔΑ</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>4626</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>04/10/2025</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1.1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>45,54</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>10,93</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>56,47</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modal summary correction v5
</commit_message>
<xml_diff>
--- a/data/excel/802576637_2025_invoices.xlsx
+++ b/data/excel/802576637_2025_invoices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,56 +489,11 @@
           <t>Σύνολο</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>issueDate</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>AFM_issuer</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>AA</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>series</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>totalNetValue</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>totalVatAmount</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>totalValue</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>character</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>400011172559639</t>
+          <t>400011184530011</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -553,17 +508,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12Μ0ΤΔΑ</t>
+          <t>5Μ0ΤΔΑ</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10768</t>
+          <t>4626</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>03/10/2025</t>
+          <t>04/10/2025</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -574,90 +529,19 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>13,83</t>
+          <t>45,54</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3,32</t>
+          <t>10,93</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>17,15</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>400011184530011</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>094439854</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>5Μ0ΤΔΑ</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>4626</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>04/10/2025</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1.1</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>45,54</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>10,93</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
           <t>56,47</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
base.html update correct fiscal year
</commit_message>
<xml_diff>
--- a/data/excel/802576637_2025_invoices.xlsx
+++ b/data/excel/802576637_2025_invoices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -695,6 +695,64 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>400011186892779</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>094439854</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>8Μ0ΤΔΑ</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>8970</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>04/10/2025</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Τιμολόγιο Πώλησης</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>48,39</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>11,61</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>60,00</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>8970</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>